<commit_message>
updated ablauf.xlsx and gantt cahrt
</commit_message>
<xml_diff>
--- a/Plannung/ablauf.xlsx
+++ b/Plannung/ablauf.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legau\Documents\1_Studium\DigitaleFabrik\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legau\Documents\1_Studium\DigitaleFabrik\Plannung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C98F2F61-B294-45E0-A9A1-D76D92F8A22E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FEB7A8-0504-4696-87BB-88BAE3288A45}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7575" yWindow="3435" windowWidth="15375" windowHeight="7875" xr2:uid="{3AE99C79-5774-4B6B-8C0B-F0FF93CACC5D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3AE99C79-5774-4B6B-8C0B-F0FF93CACC5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="56">
   <si>
     <t xml:space="preserve">Was </t>
   </si>
@@ -66,9 +66,6 @@
     <t>AID, Aufheizen1 fertig</t>
   </si>
   <si>
-    <t>AID, Maischen1, {63°C, 70 min}</t>
-  </si>
-  <si>
     <t>AID, Maischen1 fertig</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>AID, Aufheizen2 fertig</t>
   </si>
   <si>
-    <t>AID, Maischen2, {73°C, 5mnin}</t>
-  </si>
-  <si>
     <t>AID, Maischen2 fertig</t>
   </si>
   <si>
@@ -154,6 +148,57 @@
   </si>
   <si>
     <t>AID, Kühlen, {22°C}</t>
+  </si>
+  <si>
+    <t>AID, Kühlen fertig</t>
+  </si>
+  <si>
+    <t>AID, Reifen1 fertig</t>
+  </si>
+  <si>
+    <t>AID, Reifen2 fertig</t>
+  </si>
+  <si>
+    <t>AID, Hefe zugeben</t>
+  </si>
+  <si>
+    <t>AID, Hefe zugeben fertig</t>
+  </si>
+  <si>
+    <t>AID, Zucker zugeben</t>
+  </si>
+  <si>
+    <t>AID, Zucker zugeben fertig</t>
+  </si>
+  <si>
+    <t>AID, Abfüllen</t>
+  </si>
+  <si>
+    <t>AID, Abfüllen fertig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AID, RFID Tag </t>
+  </si>
+  <si>
+    <t>AID, RFID Tag fertig</t>
+  </si>
+  <si>
+    <t>AID, Auftrag abgeschlossen</t>
+  </si>
+  <si>
+    <t>SPS, Dashboard</t>
+  </si>
+  <si>
+    <t>AID, Maischen2, {73°C, 5min}</t>
+  </si>
+  <si>
+    <t>AID, Maischen1, {63°C, 70min}</t>
+  </si>
+  <si>
+    <t>AID, Reifen1, { Zimmertemperatur, 2-3 Tage}</t>
+  </si>
+  <si>
+    <t>AID, Reifen2, {5°C, 2-3 Wochen}</t>
   </si>
 </sst>
 </file>
@@ -505,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3E93B6-42C5-42F2-8BA3-B54B957CB7FA}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +591,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -571,7 +616,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -590,10 +635,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -601,7 +646,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -612,10 +657,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -623,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -634,10 +679,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -645,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -656,10 +701,10 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -667,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -678,10 +723,10 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -689,7 +734,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -700,7 +745,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -711,7 +756,7 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -722,10 +767,10 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -744,7 +789,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -755,7 +800,7 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -766,10 +811,10 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -777,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
@@ -788,7 +833,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -799,7 +844,7 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
@@ -810,10 +855,10 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -821,7 +866,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -832,7 +877,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
@@ -843,7 +888,7 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
@@ -854,10 +899,10 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -865,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
@@ -876,7 +921,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
@@ -887,7 +932,7 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -898,10 +943,164 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
         <v>40</v>
       </c>
-      <c r="C35" t="s">
-        <v>1</v>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new file for sps to sap comm and updated files
</commit_message>
<xml_diff>
--- a/Plannung/ablauf.xlsx
+++ b/Plannung/ablauf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legau\Documents\1_Studium\DigitaleFabrik\Plannung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FEB7A8-0504-4696-87BB-88BAE3288A45}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEE264B-CB90-4AD6-90A7-767AF3BBCCEE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3AE99C79-5774-4B6B-8C0B-F0FF93CACC5D}"/>
   </bookViews>
@@ -553,7 +553,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>